<commit_message>
updated arduino sample  codes i used for my PoCs
</commit_message>
<xml_diff>
--- a/IoT-Device-Buy-List.xlsx
+++ b/IoT-Device-Buy-List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A79BC9-D54C-4883-9229-83BC15A097FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A2796-5B39-4A07-AC55-AE0FDB32DFBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>https://www.amazon.in/Electrobot-Driver-Shield-Expansion-Arduino/dp/B017TZ9Q3K</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>https://www.amazon.in/REES52-R3_400-Starter-Arduino-Breadboard/dp/B01FCH95KG/</t>
+  </si>
+  <si>
+    <t>xcluma ESP32 ESP-32 ESP-32S ESP 32 Development Board CP2102 Wifi Bluetooth Ultra-Low Power Consumption Dual Core</t>
+  </si>
+  <si>
+    <t>SquadPixel ESP-32 WiFi , Bluetooth, Dual Core Chip Development Board</t>
+  </si>
+  <si>
+    <t>ESP32 Development Board CP2102 WiFi Bluetooth</t>
+  </si>
+  <si>
+    <t>ElectroBot 4 Wheel Robot Smart Car Chassis Kits Car with Speed Encoder for Arduino</t>
   </si>
 </sst>
 </file>
@@ -522,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,26 +774,34 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>

</xml_diff>